<commit_message>
added vote counts and winners to circuits xlsx and json
</commit_message>
<xml_diff>
--- a/list_scripts/okregi.xlsx
+++ b/list_scripts/okregi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.borowski\voter-trip\list_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4EDFA6-5507-40AA-8321-3B95B365C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A12847D-257D-41DF-9EB9-4ECFFF1A456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8846FECE-449A-4B59-A6F7-A071FA2F18B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>LM</t>
   </si>
@@ -303,13 +303,25 @@
   </si>
   <si>
     <t>city_name</t>
+  </si>
+  <si>
+    <t>votes_ko_2019</t>
+  </si>
+  <si>
+    <t>votes_pis_2019</t>
+  </si>
+  <si>
+    <t>swing_factor</t>
+  </si>
+  <si>
+    <t>2019_winner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,13 +341,6 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -372,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -407,36 +412,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFA2A9B1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA2A9B1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -497,24 +472,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,10 +800,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9516E671-C7C4-4CEB-9766-0B6CF91E12A3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,9 +812,13 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="94.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -860,1080 +834,1666 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="I1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>986879</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>12</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>82240</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>51.207006700000001</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>16.1553231</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="I2" s="7">
+        <v>108191</v>
+      </c>
+      <c r="J2" s="7">
+        <v>183364</v>
+      </c>
+      <c r="K2">
+        <f>IF(I2 &gt; J2,I2/J2,J2/I2)</f>
+        <v>1.694817498682885</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(I2 &gt; J2,"party_ko","party_pis")</f>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>675332</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>8</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>84417</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>50.7840092</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>16.284355300000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="I3" s="7">
+        <v>90812</v>
+      </c>
+      <c r="J3" s="7">
+        <v>114728</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K42" si="0">IF(I3 &gt; J3,I3/J3,J3/I3)</f>
+        <v>1.2633572655596177</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L42" si="1">IF(I3 &gt; J3,"party_ko","party_pis")</f>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>1177802</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>14</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>84129</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>51.107885199999998</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>17.038537600000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="I4" s="7">
+        <v>214629</v>
+      </c>
+      <c r="J4" s="7">
+        <v>226915</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>1.0572429634392371</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>1003261</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>12</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>83605</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>53.123480399999998</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>18.008437799999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="I5" s="7">
+        <v>142844</v>
+      </c>
+      <c r="J5" s="7">
+        <v>167550</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1.1729579121279157</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>1046849</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>13</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>80527</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>53.013790200000003</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>18.598443700000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="I6" s="7">
+        <v>119526</v>
+      </c>
+      <c r="J6" s="7">
+        <v>182648</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>1.5281026722219433</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>1199999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>15</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>80000</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>51.246453600000002</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>22.568446300000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="I7" s="7">
+        <v>109185</v>
+      </c>
+      <c r="J7" s="7">
+        <v>313284</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>2.8692952328616568</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>974707</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>12</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>81226</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>51.143123199999998</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>23.471198600000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="I8" s="7">
+        <v>59401</v>
+      </c>
+      <c r="J8" s="7">
+        <v>238802</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>4.0201680106395514</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>1003220</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>12</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>83602</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>51.935621400000002</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>15.5061862</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="I9" s="7">
+        <v>136955</v>
+      </c>
+      <c r="J9" s="7">
+        <v>150188</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>1.096622978350553</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>794636</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>10</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>79464</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>51.759248499999998</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>19.4559833</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="I10" s="7">
+        <v>148830</v>
+      </c>
+      <c r="J10" s="7">
+        <v>136731</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1.0884876143668956</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>party_ko</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>737045</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <v>9</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>81894</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>51.405172100000001</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>19.7030244</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="I11" s="7">
+        <v>54160</v>
+      </c>
+      <c r="J11" s="7">
+        <v>194658</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>3.594128508124077</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>972481</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>81040</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>51.5956014</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>18.7302994</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="I12" s="7">
+        <v>94268</v>
+      </c>
+      <c r="J12" s="7">
+        <v>229245</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2.4318432553994991</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>642662</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>8</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>80333</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>50.135492800000002</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <v>19.402070999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="I13" s="7">
+        <v>72869</v>
+      </c>
+      <c r="J13" s="7">
+        <v>169106</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>2.3206850649796209</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>1120711</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>14</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <v>80051</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>50.064650100000001</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="3">
         <v>19.9449799</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="I14" s="7">
+        <v>197930</v>
+      </c>
+      <c r="J14" s="7">
+        <v>256847</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1.2976658414591018</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>784316</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="6">
         <v>10</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <v>78432</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="3">
         <v>49.617453500000003</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="3">
         <v>20.7153326</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="I15" s="7">
+        <v>51183</v>
+      </c>
+      <c r="J15" s="7">
+        <v>243583</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>4.7590606255983436</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="6">
         <v>719037</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="6">
         <v>9</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <v>79893</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="3">
         <v>50.012101100000002</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="3">
         <v>20.985840700000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="I16" s="7">
+        <v>48597</v>
+      </c>
+      <c r="J16" s="7">
+        <v>206845</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>4.2563326954338745</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="6">
         <v>842976</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>10</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <v>84298</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="3">
         <v>52.546344599999998</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="3">
         <v>19.706536400000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="I17" s="7">
+        <v>62429</v>
+      </c>
+      <c r="J17" s="7">
+        <v>194371</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>3.1134729052203305</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="6">
         <v>724756</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="6">
         <v>9</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="6">
         <v>80528</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="3">
         <v>51.402723600000002</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="3">
         <v>21.1471333</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="I18" s="7">
+        <v>57449</v>
+      </c>
+      <c r="J18" s="7">
+        <v>193709</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>3.3718428519208343</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="6">
         <v>960655</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="6">
         <v>12</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="6">
         <v>80055</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="3">
         <v>52.167603100000001</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="3">
         <v>22.290164499999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="I19" s="7">
+        <v>63124</v>
+      </c>
+      <c r="J19" s="7">
+        <v>270641</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>4.2874500982193782</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <v>1603233</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>20</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>80055</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="3">
         <v>52.2296756</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="3">
         <v>21.012228700000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="I20" s="7">
+        <v>581077</v>
+      </c>
+      <c r="J20" s="7">
+        <v>379880</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1.5296330420132673</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>party_ko</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <v>986074</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <v>12</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="6">
         <v>82173</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="3">
         <v>52.2296756</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="3">
         <v>21.012228700000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="I21" s="7">
+        <v>171286</v>
+      </c>
+      <c r="J21" s="7">
+        <v>244823</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>1.4293228868675782</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="6">
         <v>1001827</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="6">
         <v>12</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="6">
         <v>83486</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="3">
         <v>50.6683223</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="3">
         <v>17.923065099999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="I22" s="7">
+        <v>108570</v>
+      </c>
+      <c r="J22" s="7">
+        <v>152999</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>1.4092198581560285</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>893055</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>11</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>81187</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="3">
         <v>49.682476100000002</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="3">
         <v>21.766053100000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="I23" s="7">
+        <v>62246</v>
+      </c>
+      <c r="J23" s="7">
+        <v>247488</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>3.9759663271535519</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="6">
         <v>1233497</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="6">
         <v>15</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="6">
         <v>82233</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="3">
         <v>50.041186699999997</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="3">
         <v>21.9991196</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="I24" s="7">
+        <v>84703</v>
+      </c>
+      <c r="J24" s="7">
+        <v>367268</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>4.3359503205317402</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="6">
         <v>1190510</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="6">
         <v>14</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="6">
         <v>85036</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="3">
         <v>53.132488600000002</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="3">
         <v>23.168840299999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="I25" s="7">
+        <v>109527</v>
+      </c>
+      <c r="J25" s="7">
+        <v>270888</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>2.4732531704511218</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="6">
         <v>1026157</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>12</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="6">
         <v>85513</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="3">
         <v>54.3520252</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="3">
         <v>18.646638400000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="I26" s="7">
+        <v>218484</v>
+      </c>
+      <c r="J26" s="7">
+        <v>169753</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>1.287070037053837</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="1"/>
+        <v>party_ko</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <v>1178950</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="6">
         <v>14</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <v>84211</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="3">
         <v>54.518889799999997</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="3">
         <v>18.530540899999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="I27" s="7">
+        <v>208208</v>
+      </c>
+      <c r="J27" s="7">
+        <v>211582</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>1.0162049488972567</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="6">
         <v>756208</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <v>9</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <v>84023</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="3">
         <v>49.822376800000001</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="3">
         <v>19.058384499999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="I28" s="7">
+        <v>105876</v>
+      </c>
+      <c r="J28" s="7">
+        <v>182027</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>1.7192470437115115</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="6">
         <v>600225</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="6">
         <v>7</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>85746</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="3">
         <v>50.811819499999999</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="3">
         <v>19.1203094</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="I29" s="7">
+        <v>64374</v>
+      </c>
+      <c r="J29" s="7">
+        <v>125990</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>1.9571566160251033</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>771169</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="6">
         <v>9</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="6">
         <v>85685</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="3">
         <v>50.294492300000002</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="3">
         <v>18.671380200000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="I30" s="7">
+        <v>111078</v>
+      </c>
+      <c r="J30" s="7">
+        <v>128579</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1.1575559516735987</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="6">
         <v>718360</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="6">
         <v>9</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <v>79818</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="3">
         <v>50.1021742</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="3">
         <v>18.546284700000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="I31" s="7">
+        <v>92493</v>
+      </c>
+      <c r="J31" s="7">
+        <v>161160</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>1.7424021277285848</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="6">
         <v>980996</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="6">
         <v>12</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="6">
         <v>81750</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="3">
         <v>50.264891900000002</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="3">
         <v>19.023781499999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="I32" s="7">
+        <v>174683</v>
+      </c>
+      <c r="J32" s="7">
+        <v>184030</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>1.0535083551347297</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="6">
         <v>700234</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="6">
         <v>9</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="6">
         <v>77804</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="3">
         <v>50.277987400000001</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="3">
         <v>19.126800200000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="I33" s="7">
+        <v>99499</v>
+      </c>
+      <c r="J33" s="7">
+        <v>124553</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>1.2518015256434738</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="6">
         <v>1283669</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="6">
         <v>16</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="6">
         <v>80229</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="3">
         <v>50.866077300000001</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="3">
         <v>20.628567700000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="I34" s="7">
+        <v>94880</v>
+      </c>
+      <c r="J34" s="7">
+        <v>314455</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>3.3142390387858347</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="6">
         <v>641373</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="6">
         <v>8</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="6">
         <v>80172</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="3">
         <v>54.156061299999998</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="3">
         <v>19.404489699999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="I35" s="7">
+        <v>71320</v>
+      </c>
+      <c r="J35" s="7">
+        <v>102478</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>1.4368760515984296</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="6">
         <v>797764</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="6">
         <v>10</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="6">
         <v>79776</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="3">
         <v>53.778421999999999</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="3">
         <v>20.480119299999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="I36" s="7">
+        <v>87780</v>
+      </c>
+      <c r="J36" s="7">
+        <v>128760</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>1.4668489405331511</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="6">
         <v>999418</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="6">
         <v>12</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="6">
         <v>83285</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="3">
         <v>51.767279899999998</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="3">
         <v>18.0853462</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="I37" s="7">
+        <v>113489</v>
+      </c>
+      <c r="J37" s="7">
+        <v>195053</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>1.7186952039404699</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="6">
         <v>773727</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="6">
         <v>9</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="6">
         <v>85970</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="3">
         <v>52.223033399999998</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="3">
         <v>18.2510729</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="I38" s="7">
+        <v>72295</v>
+      </c>
+      <c r="J38" s="7">
+        <v>166965</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>2.309495815754893</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="6">
         <v>772319</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="6">
         <v>9</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="6">
         <v>85813</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="3">
         <v>53.150967100000003</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="3">
         <v>16.738226600000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="I39" s="7">
+        <v>106810</v>
+      </c>
+      <c r="J39" s="7">
+        <v>124392</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>1.1646100552382737</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="6">
         <v>834183</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="6">
         <v>10</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="6">
         <v>83418</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="3">
         <v>52.406374</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="3">
         <v>16.9251681</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+      <c r="I40" s="7">
+        <v>233474</v>
+      </c>
+      <c r="J40" s="7">
+        <v>130319</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>1.7915576393311796</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="1"/>
+        <v>party_ko</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="6">
         <v>644377</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="6">
         <v>8</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="6">
         <v>80547</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="3">
         <v>54.194321899999998</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="3">
         <v>16.171490800000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="I41" s="7">
+        <v>87799</v>
+      </c>
+      <c r="J41" s="7">
+        <v>100078</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>1.1398535290834748</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="1"/>
+        <v>party_pis</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="6">
         <v>1026640</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="6">
         <v>12</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="6">
         <v>85553</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="3">
         <v>53.4285438</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="3">
         <v>14.5528116</v>
+      </c>
+      <c r="I42" s="7">
+        <v>168022</v>
+      </c>
+      <c r="J42" s="7">
+        <v>165200</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>1.0170823244552059</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="1"/>
+        <v>party_ko</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created navbar, swinginfo, 'go to list' button
</commit_message>
<xml_diff>
--- a/list_scripts/okregi.xlsx
+++ b/list_scripts/okregi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.borowski\voter-trip\list_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8630BB51-0176-45F6-9111-BB1B3A368CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B388D40-512C-4837-AF04-ED8FCBECBA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8846FECE-449A-4B59-A6F7-A071FA2F18B8}"/>
   </bookViews>
@@ -299,9 +299,6 @@
     <t>swing_factor</t>
   </si>
   <si>
-    <t>2019_winner</t>
-  </si>
-  <si>
     <t>residents</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>winner_2019</t>
   </si>
 </sst>
 </file>
@@ -802,8 +802,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,11 +811,11 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="94.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -830,19 +830,19 @@
         <v>81</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>84</v>
@@ -854,7 +854,7 @@
         <v>86</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1597,10 +1597,10 @@
         <v>80055</v>
       </c>
       <c r="G20" s="3">
-        <v>52.2296756</v>
+        <v>52.15</v>
       </c>
       <c r="H20" s="3">
-        <v>21.012228700000001</v>
+        <v>21.1</v>
       </c>
       <c r="I20" s="7">
         <v>581077</v>

</xml_diff>